<commit_message>
list of calibrations runnning
</commit_message>
<xml_diff>
--- a/Code/final option calibration/szenariolist.xlsx
+++ b/Code/final option calibration/szenariolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\final option calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F300405C-4386-40B3-847C-462DEFBFC6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A8FA8C-C967-4A05-83C5-9F73980D7984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="345" yWindow="1275" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,11 +483,29 @@
       <c r="A6">
         <v>2014</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -510,14 +528,14 @@
       </c>
       <c r="B13">
         <f>SUM(B2:D10)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>27</v>
       </c>
       <c r="D13" s="1">
         <f>B13/C13</f>
-        <v>0.44444444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataset generator full update
</commit_message>
<xml_diff>
--- a/Code/final option calibration/szenariolist.xlsx
+++ b/Code/final option calibration/szenariolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\final option calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A8FA8C-C967-4A05-83C5-9F73980D7984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0695C6B-16CC-43C3-8AAD-35FC61746BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="1275" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>optll</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve">total </t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -404,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C644853-D4AB-442F-AC6C-55E47ADFC711}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -422,120 +431,258 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2010</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2011</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2012</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2013</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2014</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <f>SUM(B2:D10)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>27</v>
       </c>
       <c r="D13" s="1">
         <f>B13/C13</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f>SUM(G2:I10)</f>
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>27</v>
+      </c>
+      <c r="I13" s="1">
+        <f>G13/H13</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f>B13+G13</f>
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15/C15</f>
+        <v>0.88888888888888884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better structure, just renaming and sorting
</commit_message>
<xml_diff>
--- a/Code/final option calibration/szenariolist.xlsx
+++ b/Code/final option calibration/szenariolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\final option calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0695C6B-16CC-43C3-8AAD-35FC61746BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C3995-613E-4F7C-8EC6-4FB75256F8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1275" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="9060" yWindow="2355" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>optll</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>done</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -416,7 +413,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,14 +572,14 @@
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="F7">
         <v>2015</v>
@@ -593,16 +590,25 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>2016</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -610,16 +616,22 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>2017</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -633,10 +645,13 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>2018</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -645,28 +660,28 @@
       </c>
       <c r="B13">
         <f>SUM(B2:D10)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>27</v>
       </c>
       <c r="D13" s="1">
         <f>B13/C13</f>
-        <v>0.33333333333333331</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="G13">
         <f>SUM(G2:I10)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H13">
         <v>27</v>
       </c>
       <c r="I13" s="1">
         <f>G13/H13</f>
-        <v>0.55555555555555558</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,14 +690,14 @@
       </c>
       <c r="B15">
         <f>B13+G13</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>27</v>
       </c>
       <c r="D15" s="1">
         <f>B15/C15</f>
-        <v>0.88888888888888884</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>